<commit_message>
Fait interface des capteurs principaux.
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6654DF-437D-4D2B-AB91-50295BB45179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1568D631-DA7A-4AEF-A830-742B620F71E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +550,7 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" cm="1">
@@ -571,7 +571,7 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
@@ -746,10 +746,12 @@
     <hyperlink ref="E5" r:id="rId1" xr:uid="{52282ACD-8AAF-4855-9C6E-AE457709EA21}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{83F98DBF-BD15-49DB-8E82-BFB4BC370CF5}"/>
     <hyperlink ref="E7" r:id="rId3" display="https://www.digikey.ca/en/products/detail/sunfounder/CN0296D/18668625?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-18668625_sig-Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB" xr:uid="{F76E9493-DB9B-4C1B-877C-79A2F0469D72}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{A1B2DE21-05A5-4969-8B26-9E80459322CD}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{D6230C34-D026-4A11-92B9-B3EBC45F1587}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finir layout schematic et création projet firmware pour rfreceiver
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1568D631-DA7A-4AEF-A830-742B620F71E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E198A4D6-C18A-4E2D-B3E0-0326EECFEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,7 +591,7 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
@@ -748,10 +748,11 @@
     <hyperlink ref="E7" r:id="rId3" display="https://www.digikey.ca/en/products/detail/sunfounder/CN0296D/18668625?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-18668625_sig-Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB" xr:uid="{F76E9493-DB9B-4C1B-877C-79A2F0469D72}"/>
     <hyperlink ref="E2" r:id="rId4" xr:uid="{A1B2DE21-05A5-4969-8B26-9E80459322CD}"/>
     <hyperlink ref="E3" r:id="rId5" xr:uid="{D6230C34-D026-4A11-92B9-B3EBC45F1587}"/>
+    <hyperlink ref="E4" r:id="rId6" display="https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB" xr:uid="{153A9C95-770B-40E2-BD79-ADD1965FFD45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changement régulateurs, meilleur circuit debouncing boutons, documentation
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E198A4D6-C18A-4E2D-B3E0-0326EECFEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25E0066-E549-47D2-BB7D-C6EE01B6FF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>MLX90393</t>
   </si>
@@ -102,24 +102,12 @@
     <t>https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB</t>
   </si>
   <si>
-    <t>AP2210</t>
-  </si>
-  <si>
     <t>régulateur 5V</t>
   </si>
   <si>
     <t>régulateur 3,3V</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/diodes-incorporated/AP2210N-3-3TRG1/4470822</t>
-  </si>
-  <si>
-    <t>LP2980</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/texas-instruments/LP2980AIM5-5-0-NOPB/334966</t>
-  </si>
-  <si>
     <t>CN0296D</t>
   </si>
   <si>
@@ -135,31 +123,40 @@
     <t>.</t>
   </si>
   <si>
-    <t>RF2-04A-T-00-50-G</t>
-  </si>
-  <si>
     <t>connecteur SMA</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/adam-tech/RF2-04A-T-00-50-G/9830588</t>
-  </si>
-  <si>
-    <t>SMTB-0927-TW-R</t>
-  </si>
-  <si>
     <t>buzzer</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/pui-audio-inc/SMTB-0927-TW-R/13165907</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/wurth-electronics-inc/150080GS75000/4489913?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2qjWmhU0NNvxIPN9v6GT5Pp73s1ZT1kcE5agLq5cV6UoWDQ3-2epNEaAr57EALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2qjWmhU0NNvxIPN9v6GT5Pp73s1ZT1kcE5agLq5cV6UoWDQ3-2epNEaAr57EALw_wcB</t>
-  </si>
-  <si>
     <t>led verte</t>
   </si>
   <si>
-    <t>150080GS75000</t>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/NCV5501DT33RKG/1792725</t>
+  </si>
+  <si>
+    <t>I (mA)</t>
+  </si>
+  <si>
+    <t>led rouge</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/liteon/LTST-C190EKT/269229?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C170GKT/269226</t>
+  </si>
+  <si>
+    <t>bouton</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/nisshinbo-micro-devices-inc/NJM2882F05-TE1/10671911</t>
+  </si>
+  <si>
+    <t>NJM2882F05</t>
+  </si>
+  <si>
+    <t>NCV5501DT33RKG</t>
   </si>
 </sst>
 </file>
@@ -226,10 +223,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:F28" totalsRowShown="0">
-  <autoFilter ref="A1:F28" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:G28" totalsRowShown="0">
+  <autoFilter ref="A1:G28" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CFC39690-F582-4CE4-97DA-17BB86A09181}" name="NOM"/>
+    <tableColumn id="7" xr3:uid="{079D81A1-266A-4698-9F00-BD6970F9F3EB}" name="I (mA)"/>
     <tableColumn id="2" xr3:uid="{587DB22B-B42F-4EDD-807E-A98F888AAC49}" name="QTE"/>
     <tableColumn id="3" xr3:uid="{C4D9BA48-319C-429D-9D6D-77D5CE4E5FAC}" name="PRIX"/>
     <tableColumn id="4" xr3:uid="{1F48FE55-C008-466A-91A1-B0574400C635}" name="DESCRIPTION"/>
@@ -503,252 +501,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>1.75</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2.85</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" cm="1">
-        <f t="array" ref="F2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>85.72999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" cm="1">
+        <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
+        <v>82.070000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
+        <v>18.5</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>18.52</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>17.329999999999998</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>-500</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1.53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>0.72</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D7">
+        <v>20.82</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6">
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>1.03</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>20.82</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>3.83</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>0.24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0.34</v>
+      </c>
+      <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1.27</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
-        <v>24</v>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{52282ACD-8AAF-4855-9C6E-AE457709EA21}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{83F98DBF-BD15-49DB-8E82-BFB4BC370CF5}"/>
-    <hyperlink ref="E7" r:id="rId3" display="https://www.digikey.ca/en/products/detail/sunfounder/CN0296D/18668625?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-18668625_sig-Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB" xr:uid="{F76E9493-DB9B-4C1B-877C-79A2F0469D72}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{A1B2DE21-05A5-4969-8B26-9E80459322CD}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{D6230C34-D026-4A11-92B9-B3EBC45F1587}"/>
-    <hyperlink ref="E4" r:id="rId6" display="https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB" xr:uid="{153A9C95-770B-40E2-BD79-ADD1965FFD45}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{52282ACD-8AAF-4855-9C6E-AE457709EA21}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{83F98DBF-BD15-49DB-8E82-BFB4BC370CF5}"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.digikey.ca/en/products/detail/sunfounder/CN0296D/18668625?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-18668625_sig-Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjw7Py4BhCbARIsAMMx-_IbWQh40LwBNp9m3tWvmAtQJ6C_7EYDRPz0lulxMv0K1667RdN-usYaAnGWEALw_wcB" xr:uid="{F76E9493-DB9B-4C1B-877C-79A2F0469D72}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{A1B2DE21-05A5-4969-8B26-9E80459322CD}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{D6230C34-D026-4A11-92B9-B3EBC45F1587}"/>
+    <hyperlink ref="F4" r:id="rId6" display="https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB" xr:uid="{153A9C95-770B-40E2-BD79-ADD1965FFD45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
choix ferrite bead et footprint
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25E0066-E549-47D2-BB7D-C6EE01B6FF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B82B14-86E8-4422-AC38-A7E1F1DB1DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>MLX90393</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>NCV5501DT33RKG</t>
+  </si>
+  <si>
+    <t>ferrite bead</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/ILBB0603ER121V/2574888</t>
+  </si>
+  <si>
+    <t>ILBB0603ER121V</t>
+  </si>
+  <si>
+    <t>LTST-C170GKT</t>
+  </si>
+  <si>
+    <t>LTST-C190EKT</t>
   </si>
 </sst>
 </file>
@@ -501,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,7 +575,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>82.070000000000007</v>
+        <v>82.23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -701,6 +716,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
       <c r="B10">
         <v>10</v>
       </c>
@@ -713,7 +731,7 @@
       <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G10" t="s">
@@ -721,6 +739,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
       <c r="B11">
         <v>10</v>
       </c>
@@ -733,7 +754,7 @@
       <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G11" t="s">
@@ -755,12 +776,25 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0.16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -772,10 +806,12 @@
     <hyperlink ref="F2" r:id="rId4" xr:uid="{A1B2DE21-05A5-4969-8B26-9E80459322CD}"/>
     <hyperlink ref="F3" r:id="rId5" xr:uid="{D6230C34-D026-4A11-92B9-B3EBC45F1587}"/>
     <hyperlink ref="F4" r:id="rId6" display="https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB" xr:uid="{153A9C95-770B-40E2-BD79-ADD1965FFD45}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{A217C864-8D85-4E7F-8E31-A6D000832483}"/>
+    <hyperlink ref="F11" r:id="rId8" display="https://www.digikey.ca/en/products/detail/liteon/LTST-C190EKT/269229?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE" xr:uid="{52AEB8C1-3281-4CF0-B9F2-15F673CB6E65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Choix cristal 8MHz et Connecteur SMA. Footprint et documentation
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B82B14-86E8-4422-AC38-A7E1F1DB1DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9252C53E-C8AD-466B-BA1B-1D6C54A18D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>MLX90393</t>
   </si>
@@ -172,6 +172,24 @@
   </si>
   <si>
     <t>LTST-C190EKT</t>
+  </si>
+  <si>
+    <t>YG8M000000S418</t>
+  </si>
+  <si>
+    <t>Cristal 8MHz</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/nextgen-components/YG8M000000S418/17289334</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adam-tech/RF2-03E-T-00-50-G/9831386</t>
+  </si>
+  <si>
+    <t>RF2-03E-T-00-50-G</t>
+  </si>
+  <si>
+    <t>Connecteur SMA 90deg</t>
   </si>
 </sst>
 </file>
@@ -516,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,7 +593,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>82.23</v>
+        <v>88.27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -795,6 +813,46 @@
         <v>34</v>
       </c>
       <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1.85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Buzzer et diode. Toutes les pièces importantes sont choisies et footprint
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9252C53E-C8AD-466B-BA1B-1D6C54A18D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D95E80-640E-4E26-AB84-BF948178BDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>MLX90393</t>
   </si>
@@ -123,9 +123,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>connecteur SMA</t>
-  </si>
-  <si>
     <t>buzzer</t>
   </si>
   <si>
@@ -190,6 +187,27 @@
   </si>
   <si>
     <t>Connecteur SMA 90deg</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/pui-audio-inc/SMTB-0927-TW-R/13165907</t>
+  </si>
+  <si>
+    <t>SMTB-0927-TW-R</t>
+  </si>
+  <si>
+    <t>TL1105T</t>
+  </si>
+  <si>
+    <t>interrupteur on/off</t>
+  </si>
+  <si>
+    <t>potentiomètre</t>
+  </si>
+  <si>
+    <t>RK09K1130</t>
+  </si>
+  <si>
+    <t>7000toggle</t>
   </si>
 </sst>
 </file>
@@ -256,8 +274,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:G28" totalsRowShown="0">
-  <autoFilter ref="A1:G28" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:G29" totalsRowShown="0">
+  <autoFilter ref="A1:G29" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CFC39690-F582-4CE4-97DA-17BB86A09181}" name="NOM"/>
     <tableColumn id="7" xr3:uid="{079D81A1-266A-4698-9F00-BD6970F9F3EB}" name="I (mA)"/>
@@ -534,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +572,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -593,7 +611,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>88.27</v>
+        <v>89.539999999999992</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -644,7 +662,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>-500</v>
@@ -659,7 +677,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -667,7 +685,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>300</v>
@@ -682,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
@@ -712,22 +730,46 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>80</v>
+      </c>
       <c r="C8">
         <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1.27</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
       </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
       <c r="G8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.24</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -741,16 +783,16 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0.24</v>
+        <v>0.34</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -758,59 +800,40 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>0.34</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>6</v>
+      <c r="A12" t="s">
+        <v>48</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B13">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0.16</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -818,19 +841,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>150</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1.85</v>
+        <v>0.16</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
@@ -838,21 +864,41 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1.85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -864,8 +910,8 @@
     <hyperlink ref="F2" r:id="rId4" xr:uid="{A1B2DE21-05A5-4969-8B26-9E80459322CD}"/>
     <hyperlink ref="F3" r:id="rId5" xr:uid="{D6230C34-D026-4A11-92B9-B3EBC45F1587}"/>
     <hyperlink ref="F4" r:id="rId6" display="https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB" xr:uid="{153A9C95-770B-40E2-BD79-ADD1965FFD45}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{A217C864-8D85-4E7F-8E31-A6D000832483}"/>
-    <hyperlink ref="F11" r:id="rId8" display="https://www.digikey.ca/en/products/detail/liteon/LTST-C190EKT/269229?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE" xr:uid="{52AEB8C1-3281-4CF0-B9F2-15F673CB6E65}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{A217C864-8D85-4E7F-8E31-A6D000832483}"/>
+    <hyperlink ref="F10" r:id="rId8" display="https://www.digikey.ca/en/products/detail/liteon/LTST-C190EKT/269229?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE" xr:uid="{52AEB8C1-3281-4CF0-B9F2-15F673CB6E65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Footprint et choix composantes mineures (résistances et condo)
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D95E80-640E-4E26-AB84-BF948178BDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117AC510-CA75-485F-BD39-F63805CAA42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
   <si>
     <t>MLX90393</t>
   </si>
@@ -208,6 +208,93 @@
   </si>
   <si>
     <t>7000toggle</t>
+  </si>
+  <si>
+    <t>res 10k</t>
+  </si>
+  <si>
+    <t>res 1k5</t>
+  </si>
+  <si>
+    <t>cond 4,7u</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/cal-chip-electronics-inc/GMC10X7R475K10NT/24343641</t>
+  </si>
+  <si>
+    <t>cond 10u</t>
+  </si>
+  <si>
+    <t>cond 1u</t>
+  </si>
+  <si>
+    <t>cond 100n</t>
+  </si>
+  <si>
+    <t>cond 10n</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/venkel/AGC1206X6S250-106KXE/20484934</t>
+  </si>
+  <si>
+    <t>1206(3216)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/venkel/AGC0603X7R250-105KXP/20484944</t>
+  </si>
+  <si>
+    <t>0603(1608)</t>
+  </si>
+  <si>
+    <t>0402(1005)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/venkel/AGC0402X7R500-104KNP/21783535</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/venkel/AGC0402X7R500-103KNP/20484952</t>
+  </si>
+  <si>
+    <t>res 2k</t>
+  </si>
+  <si>
+    <t>cond 16p</t>
+  </si>
+  <si>
+    <t>res 145 (50mA)</t>
+  </si>
+  <si>
+    <t>res 30 (100mA)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW120630R0FKEAHP/2227586</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/koa-speer-electronics-inc/RN73H2BTTD1450F100/10092754</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW1206330RFKEAHP/2227698</t>
+  </si>
+  <si>
+    <t>res 330 (50mA)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0402JR-0710KL/726418</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC1206FR-072KL/728612</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERA-8AEB152V/3070810</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/kyocera-avx/04025U160FAT2A/3079962</t>
+  </si>
+  <si>
+    <t>cond C</t>
+  </si>
+  <si>
+    <t>res R</t>
   </si>
 </sst>
 </file>
@@ -274,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:G29" totalsRowShown="0">
-  <autoFilter ref="A1:G29" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:G38" totalsRowShown="0">
+  <autoFilter ref="A1:G38" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CFC39690-F582-4CE4-97DA-17BB86A09181}" name="NOM"/>
     <tableColumn id="7" xr3:uid="{079D81A1-266A-4698-9F00-BD6970F9F3EB}" name="I (mA)"/>
@@ -552,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,7 +698,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>89.539999999999992</v>
+        <v>95.137669999999986</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -875,7 +962,7 @@
       <c r="E15" t="s">
         <v>38</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G15" t="s">
@@ -899,6 +986,308 @@
         <v>40</v>
       </c>
       <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>9.3060000000000004E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>1.806E-2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>8.0499999999999999E-3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1.8600000000000001E-3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>0.33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>0.1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>0.1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0.27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>0.39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>0.39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
         <v>20</v>
       </c>
     </row>
@@ -912,10 +1301,13 @@
     <hyperlink ref="F4" r:id="rId6" display="https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB" xr:uid="{153A9C95-770B-40E2-BD79-ADD1965FFD45}"/>
     <hyperlink ref="F9" r:id="rId7" xr:uid="{A217C864-8D85-4E7F-8E31-A6D000832483}"/>
     <hyperlink ref="F10" r:id="rId8" display="https://www.digikey.ca/en/products/detail/liteon/LTST-C190EKT/269229?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE" xr:uid="{52AEB8C1-3281-4CF0-B9F2-15F673CB6E65}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{4840CE78-288C-43B8-8AAE-EBD5F3CCF74D}"/>
+    <hyperlink ref="F21" r:id="rId10" xr:uid="{D384BA1F-9224-4509-8533-B710B5F9084C}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{365D7651-3F25-46BE-BEB6-8284AFBEBA76}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Début PCB. Groupement et placement des composantes.
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F96F08-45F9-4B63-B524-2446912E6FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDACCE4-1BAA-4CE1-BE63-E2A1669364EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-11310" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,12 +282,6 @@
     <t>https://www.digikey.ca/en/products/detail/yageo/RC0402JR-0710KL/726418</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/RC1206FR-072KL/728612</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERA-8AEB152V/3070810</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/kyocera-avx/04025U160FAT2A/3079962</t>
   </si>
   <si>
@@ -295,6 +289,12 @@
   </si>
   <si>
     <t>res R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERA-2AEB152X/1706009</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERJ-2RKF2001X/192194</t>
   </si>
 </sst>
 </file>
@@ -642,7 +642,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +698,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>95.137669999999986</v>
+        <v>94.717669999999984</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1102,7 +1102,7 @@
         <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
@@ -1116,7 +1116,7 @@
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H24" t="s">
         <v>62</v>
@@ -1158,13 +1158,13 @@
         <v>65</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G27" t="s">
         <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
@@ -1192,19 +1192,19 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>0.39</v>
+        <v>0.18</v>
       </c>
       <c r="E29" t="s">
         <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G29" t="s">
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
suggestions de Luca et placement sur PCB
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDACCE4-1BAA-4CE1-BE63-E2A1669364EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48656FB4-78A6-43A7-A801-1AF068F6B86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-11310" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
   <si>
     <t>MLX90393</t>
   </si>
@@ -273,19 +273,10 @@
     <t>https://www.digikey.ca/en/products/detail/koa-speer-electronics-inc/RN73H2BTTD1450F100/10092754</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW1206330RFKEAHP/2227698</t>
-  </si>
-  <si>
-    <t>res 330 (50mA)</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/yageo/RC0402JR-0710KL/726418</t>
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/kyocera-avx/04025U160FAT2A/3079962</t>
-  </si>
-  <si>
-    <t>cond C</t>
   </si>
   <si>
     <t>res R</t>
@@ -641,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +689,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>94.717669999999984</v>
+        <v>95.247669999999985</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1102,7 +1093,7 @@
         <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
@@ -1111,17 +1102,6 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="E24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="G25" t="s">
         <v>20</v>
@@ -1129,7 +1109,7 @@
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <v>0.1</v>
@@ -1138,7 +1118,7 @@
         <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G26" t="s">
         <v>20</v>
@@ -1158,7 +1138,7 @@
         <v>65</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
         <v>20</v>
@@ -1198,7 +1178,7 @@
         <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G29" t="s">
         <v>20</v>
@@ -1209,7 +1189,7 @@
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>0.39</v>
@@ -1228,23 +1208,8 @@
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>0.24</v>
-      </c>
-      <c r="E31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" t="s">
-        <v>71</v>
-      </c>
       <c r="G31" t="s">
         <v>20</v>
-      </c>
-      <c r="H31" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.3">
@@ -1252,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
aucun changement, simplement fichiers non sauvegardés du dernier commit
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48656FB4-78A6-43A7-A801-1AF068F6B86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AF55F0-6CBC-4D1F-890E-CB226306DD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>MLX90393</t>
   </si>
@@ -207,9 +207,6 @@
     <t>RK09K1130</t>
   </si>
   <si>
-    <t>7000toggle</t>
-  </si>
-  <si>
     <t>res 10k</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t>https://www.digikey.ca/en/products/detail/venkel/AGC0402X7R500-103KNP/20484952</t>
   </si>
   <si>
-    <t>res 2k</t>
-  </si>
-  <si>
     <t>cond 16p</t>
   </si>
   <si>
@@ -285,7 +279,10 @@
     <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERA-2AEB152X/1706009</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERJ-2RKF2001X/192194</t>
+    <t>D102J12S215PQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/c-k/D102J12S215PQA/768267</t>
   </si>
 </sst>
 </file>
@@ -632,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +686,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>95.247669999999985</v>
+        <v>99.277669999999986</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -878,15 +875,23 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C11">
         <v>1</v>
+      </c>
+      <c r="D11">
+        <v>4.03</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -913,6 +918,9 @@
       <c r="E13" t="s">
         <v>28</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G13" t="s">
         <v>20</v>
       </c>
@@ -993,10 +1001,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="G18" t="s">
         <v>20</v>
@@ -1010,16 +1018,16 @@
         <v>9.3060000000000004E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="s">
         <v>58</v>
-      </c>
-      <c r="G19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.3">
@@ -1030,16 +1038,16 @@
         <v>1.806E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
         <v>60</v>
-      </c>
-      <c r="G20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.3">
@@ -1050,16 +1058,16 @@
         <v>8.0499999999999999E-3</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.3">
@@ -1070,16 +1078,16 @@
         <v>1.8600000000000001E-3</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.3">
@@ -1090,16 +1098,16 @@
         <v>0.33</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.3">
@@ -1109,42 +1117,27 @@
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D26">
         <v>0.1</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G26" t="s">
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>0.1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" t="s">
-        <v>75</v>
-      </c>
       <c r="G27" t="s">
         <v>20</v>
-      </c>
-      <c r="H27" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
@@ -1155,16 +1148,16 @@
         <v>0.27</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G28" t="s">
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.3">
@@ -1175,16 +1168,16 @@
         <v>0.18</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G29" t="s">
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
@@ -1195,16 +1188,16 @@
         <v>0.39</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.3">
@@ -1217,13 +1210,13 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.3">
@@ -1269,10 +1262,12 @@
     <hyperlink ref="F18" r:id="rId9" xr:uid="{4840CE78-288C-43B8-8AAE-EBD5F3CCF74D}"/>
     <hyperlink ref="F21" r:id="rId10" xr:uid="{D384BA1F-9224-4509-8533-B710B5F9084C}"/>
     <hyperlink ref="F15" r:id="rId11" xr:uid="{365D7651-3F25-46BE-BEB6-8284AFBEBA76}"/>
+    <hyperlink ref="F11" r:id="rId12" xr:uid="{831C648A-0ED8-4A30-A993-A074107CB4D5}"/>
+    <hyperlink ref="F13" r:id="rId13" xr:uid="{367CB230-24EA-4773-BA42-8053506BFC2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changement switch pour switch plus petite
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AF55F0-6CBC-4D1F-890E-CB226306DD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F8B3C1-2912-47EE-93E9-486A21794662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
   <si>
     <t>MLX90393</t>
   </si>
@@ -204,9 +204,6 @@
     <t>potentiomètre</t>
   </si>
   <si>
-    <t>RK09K1130</t>
-  </si>
-  <si>
     <t>res 10k</t>
   </si>
   <si>
@@ -279,10 +276,19 @@
     <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERA-2AEB152X/1706009</t>
   </si>
   <si>
-    <t>D102J12S215PQA</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/c-k/D102J12S215PQA/768267</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/c-k/L101011MS02Q/484142</t>
+  </si>
+  <si>
+    <t>L101011MS02Q</t>
+  </si>
+  <si>
+    <t>RK09K1130A5R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/alps-alpine/RK09K1130A5R/21721633</t>
   </si>
 </sst>
 </file>
@@ -629,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,7 +692,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>99.277669999999986</v>
+        <v>100.97766999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -875,19 +881,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>4.03</v>
+        <v>3.73</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -895,15 +901,23 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="C12">
         <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -919,7 +933,7 @@
         <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -1001,10 +1015,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G18" t="s">
         <v>20</v>
@@ -1018,16 +1032,16 @@
         <v>9.3060000000000004E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="s">
         <v>57</v>
-      </c>
-      <c r="G19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.3">
@@ -1038,16 +1052,16 @@
         <v>1.806E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
         <v>59</v>
-      </c>
-      <c r="G20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.3">
@@ -1058,16 +1072,16 @@
         <v>8.0499999999999999E-3</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.3">
@@ -1078,16 +1092,16 @@
         <v>1.8600000000000001E-3</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22" t="s">
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.3">
@@ -1098,16 +1112,16 @@
         <v>0.33</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.3">
@@ -1123,16 +1137,16 @@
         <v>0.1</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G26" t="s">
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
@@ -1148,16 +1162,16 @@
         <v>0.27</v>
       </c>
       <c r="E28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" t="s">
         <v>66</v>
       </c>
-      <c r="F28" t="s">
-        <v>67</v>
-      </c>
       <c r="G28" t="s">
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.3">
@@ -1168,16 +1182,16 @@
         <v>0.18</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
@@ -1188,16 +1202,16 @@
         <v>0.39</v>
       </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.3">
@@ -1210,13 +1224,13 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.3">
@@ -1262,12 +1276,11 @@
     <hyperlink ref="F18" r:id="rId9" xr:uid="{4840CE78-288C-43B8-8AAE-EBD5F3CCF74D}"/>
     <hyperlink ref="F21" r:id="rId10" xr:uid="{D384BA1F-9224-4509-8533-B710B5F9084C}"/>
     <hyperlink ref="F15" r:id="rId11" xr:uid="{365D7651-3F25-46BE-BEB6-8284AFBEBA76}"/>
-    <hyperlink ref="F11" r:id="rId12" xr:uid="{831C648A-0ED8-4A30-A993-A074107CB4D5}"/>
-    <hyperlink ref="F13" r:id="rId13" xr:uid="{367CB230-24EA-4773-BA42-8053506BFC2F}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{367CB230-24EA-4773-BA42-8053506BFC2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout annotations silkscreen et mise à jour bill of material
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F8B3C1-2912-47EE-93E9-486A21794662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4962B2-2219-4D58-BB65-F723037150B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-11310" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t>MLX90393</t>
   </si>
@@ -289,6 +289,24 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/alps-alpine/RK09K1130A5R/21721633</t>
+  </si>
+  <si>
+    <t>MMBT3904</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/MMBT3904LT1G/1139813</t>
+  </si>
+  <si>
+    <t>Transistor NPN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/BAT54T1G/918319</t>
+  </si>
+  <si>
+    <t>BAT54T1G</t>
+  </si>
+  <si>
+    <t>Diode schottky</t>
   </si>
 </sst>
 </file>
@@ -355,8 +373,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:G38" totalsRowShown="0">
-  <autoFilter ref="A1:G38" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}" name="Tableau1" displayName="Tableau1" ref="A1:G40" totalsRowShown="0">
+  <autoFilter ref="A1:G40" xr:uid="{F62023DF-2644-4AEA-B934-E5CDE90B1572}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CFC39690-F582-4CE4-97DA-17BB86A09181}" name="NOM"/>
     <tableColumn id="7" xr3:uid="{079D81A1-266A-4698-9F00-BD6970F9F3EB}" name="I (mA)"/>
@@ -633,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +666,7 @@
     <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -671,7 +689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -692,10 +710,10 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>100.97766999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101.05453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -718,7 +736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -741,7 +759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -764,7 +782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -787,7 +805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -810,7 +828,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -833,7 +851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -856,7 +874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -879,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -899,7 +917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -919,7 +937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -938,8 +956,9 @@
       <c r="G13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -962,7 +981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -982,7 +1001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -995,127 +1014,127 @@
       <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0.12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
       <c r="G17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
+        <v>0.13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
         <v>9.3060000000000004E-2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>56</v>
       </c>
-      <c r="G19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
         <v>1.806E-2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" t="s">
         <v>53</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F22" t="s">
         <v>58</v>
       </c>
-      <c r="G20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C21">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C23">
         <v>9</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>8.0499999999999999E-3</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G21" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>1.8600000000000001E-3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>0.33</v>
-      </c>
-      <c r="E23" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" t="s">
-        <v>69</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
@@ -1124,88 +1143,88 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1.8600000000000001E-3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>0.33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
       <c r="G25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26">
+      <c r="H25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
         <v>0.1</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>48</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F28" t="s">
         <v>68</v>
       </c>
-      <c r="G26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
         <v>0.27</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
         <v>65</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F30" t="s">
         <v>66</v>
-      </c>
-      <c r="G28" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>0.18</v>
-      </c>
-      <c r="E29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C30">
-        <v>7</v>
-      </c>
-      <c r="D30">
-        <v>0.39</v>
-      </c>
-      <c r="E30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" t="s">
-        <v>67</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
@@ -1214,52 +1233,92 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>0.18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>71</v>
+      </c>
       <c r="G31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C32">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>0.39</v>
       </c>
       <c r="E32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>70</v>
       </c>
-      <c r="G32" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="G34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
       <c r="G35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
       <c r="G36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
       <c r="G38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1273,14 +1332,16 @@
     <hyperlink ref="F4" r:id="rId6" display="https://www.digikey.ca/en/products/detail/stmicroelectronics/STM32F103RET6/1852094?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_GEM%20Suppliers&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21018510932_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2ofpqMmrciDNnl11WMPF3NpS7J_J1WO6VUPsyCk_IxFGBgjEznLmLYaAuYwEALw_wcB" xr:uid="{153A9C95-770B-40E2-BD79-ADD1965FFD45}"/>
     <hyperlink ref="F9" r:id="rId7" xr:uid="{A217C864-8D85-4E7F-8E31-A6D000832483}"/>
     <hyperlink ref="F10" r:id="rId8" display="https://www.digikey.ca/en/products/detail/liteon/LTST-C190EKT/269229?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE" xr:uid="{52AEB8C1-3281-4CF0-B9F2-15F673CB6E65}"/>
-    <hyperlink ref="F18" r:id="rId9" xr:uid="{4840CE78-288C-43B8-8AAE-EBD5F3CCF74D}"/>
-    <hyperlink ref="F21" r:id="rId10" xr:uid="{D384BA1F-9224-4509-8533-B710B5F9084C}"/>
+    <hyperlink ref="F20" r:id="rId9" xr:uid="{4840CE78-288C-43B8-8AAE-EBD5F3CCF74D}"/>
+    <hyperlink ref="F23" r:id="rId10" xr:uid="{D384BA1F-9224-4509-8533-B710B5F9084C}"/>
     <hyperlink ref="F15" r:id="rId11" xr:uid="{365D7651-3F25-46BE-BEB6-8284AFBEBA76}"/>
     <hyperlink ref="F13" r:id="rId12" xr:uid="{367CB230-24EA-4773-BA42-8053506BFC2F}"/>
+    <hyperlink ref="F16" r:id="rId13" xr:uid="{FB456B5E-3B77-48F7-96D1-A4E2824E9669}"/>
+    <hyperlink ref="F11" r:id="rId14" xr:uid="{3B779E7A-B4D3-41A2-96C9-36BC70E5DBEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changement circuit volume du buzzer. Ajustement du volume direct plutot que software.
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4962B2-2219-4D58-BB65-F723037150B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438A1AC9-ACBA-40AD-969C-6B0887A46D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-11310" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,12 +255,6 @@
     <t>res 145 (50mA)</t>
   </si>
   <si>
-    <t>res 30 (100mA)</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW120630R0FKEAHP/2227586</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/koa-speer-electronics-inc/RN73H2BTTD1450F100/10092754</t>
   </si>
   <si>
@@ -285,12 +279,6 @@
     <t>L101011MS02Q</t>
   </si>
   <si>
-    <t>RK09K1130A5R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/alps-alpine/RK09K1130A5R/21721633</t>
-  </si>
-  <si>
     <t>MMBT3904</t>
   </si>
   <si>
@@ -307,6 +295,18 @@
   </si>
   <si>
     <t>Diode schottky</t>
+  </si>
+  <si>
+    <t>PTV09A-4025S-A103</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/bourns-inc/PTV09A-4025S-A103/3820578</t>
+  </si>
+  <si>
+    <t>res 50 (100mA)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/TNPW120650R0BEEN/21556504?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbRBgDYAWakAXXwAcAXKEAZSYCcBLAOwHMQAX3xgYATgjQQSSGix5CJEAA4AzAHYADCrqMWkdlz6CRZHQFZ4MlBhz4ikUha0ACAPIALALaY9IZlYAVV5uJndkAFlsVEwAV05sYTM4JxBEzG5MJgJOOiEgA</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +710,7 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">SUM(Tableau1[QTE]*Tableau1[PRIX])</f>
-        <v>101.05453</v>
+        <v>100.78453</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -899,7 +899,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -911,7 +911,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -919,19 +919,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
         <v>20</v>
@@ -951,7 +951,7 @@
         <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1032,10 +1032,10 @@
         <v>0.12</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
         <v>20</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1052,10 +1052,10 @@
         <v>0.13</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G18" t="s">
         <v>20</v>
@@ -1174,7 +1174,7 @@
         <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G25" t="s">
         <v>20</v>
@@ -1199,7 +1199,7 @@
         <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G28" t="s">
         <v>20</v>
@@ -1218,13 +1218,13 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0.27</v>
+        <v>0.91</v>
       </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
@@ -1244,7 +1244,7 @@
         <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G31" t="s">
         <v>20</v>
@@ -1264,7 +1264,7 @@
         <v>64</v>
       </c>
       <c r="F32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>
@@ -1283,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34" t="s">
         <v>20</v>
@@ -1338,10 +1338,11 @@
     <hyperlink ref="F13" r:id="rId12" xr:uid="{367CB230-24EA-4773-BA42-8053506BFC2F}"/>
     <hyperlink ref="F16" r:id="rId13" xr:uid="{FB456B5E-3B77-48F7-96D1-A4E2824E9669}"/>
     <hyperlink ref="F11" r:id="rId14" xr:uid="{3B779E7A-B4D3-41A2-96C9-36BC70E5DBEB}"/>
+    <hyperlink ref="F12" r:id="rId15" xr:uid="{267E1B24-1826-4BB8-B053-1E23DB68BF16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>